<commit_message>
Save on sharepoint beginning
</commit_message>
<xml_diff>
--- a/AvanceBrico.xlsx
+++ b/AvanceBrico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\BDepBDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846EBAE5-58A3-4CF3-BF2F-66A496DC9323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77834B79-FBA0-4B15-9083-01EB6F78ED41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
+    <workbookView xWindow="32745" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateur non admin" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="523">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -1605,6 +1605,9 @@
   </si>
   <si>
     <t>Comprendre comment marche le excel</t>
+  </si>
+  <si>
+    <t>logWindow: griser pendant chargement</t>
   </si>
 </sst>
 </file>
@@ -4097,8 +4100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CCEB15-3D11-4D0A-B678-DDAB2C4259D8}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4202,7 @@
       </c>
       <c r="E5">
         <f>SUM(B:B)</f>
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -4306,11 +4309,11 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H12" t="s">
         <v>40</v>
@@ -4328,7 +4331,7 @@
       </c>
       <c r="E13" s="7">
         <f>E5/E7</f>
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
@@ -4534,10 +4537,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81565F2-C809-4864-BDA5-8C040865BE7F}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4713,6 +4716,11 @@
         <v>514</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>522</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reste l'ecriture a modifier zeubibiebiabo
</commit_message>
<xml_diff>
--- a/AvanceBrico.xlsx
+++ b/AvanceBrico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\BDepBDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E27D93E-6241-4994-A559-0F4771AF7455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4405F2-7032-4E94-92A0-560893383CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35190" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateur non admin" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="525">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -1611,6 +1611,9 @@
   </si>
   <si>
     <t>logwindow: sur entree lancer</t>
+  </si>
+  <si>
+    <t>Faire un fichier requete quand meme</t>
   </si>
 </sst>
 </file>
@@ -4540,10 +4543,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81565F2-C809-4864-BDA5-8C040865BE7F}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4729,6 +4732,11 @@
         <v>523</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>524</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AvancéeDesign, travail sur creation
</commit_message>
<xml_diff>
--- a/AvanceBrico.xlsx
+++ b/AvanceBrico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\BDepBDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FA194-A626-40D1-9FC6-648996F92EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36A86D6-4CD9-49B9-B5D9-8ACFEAA7013F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateur non admin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="560">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -1716,7 +1716,10 @@
     <t>Rechcherche enelver case sensitiv</t>
   </si>
   <si>
-    <t>Centrer le tout</t>
+    <t>Mieux gerer le centrage en haut</t>
+  </si>
+  <si>
+    <t>upgrade</t>
   </si>
 </sst>
 </file>
@@ -4680,7 +4683,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4722,10 +4725,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>532</v>
       </c>
       <c r="D2">
@@ -4734,10 +4737,10 @@
       <c r="E2" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>539</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -4751,13 +4754,16 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>559</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>533</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>538</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -4771,7 +4777,7 @@
       <c r="D4" t="s">
         <v>546</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>545</v>
       </c>
       <c r="K4" t="s">

</xml_diff>

<commit_message>
Travail format tableau etc
</commit_message>
<xml_diff>
--- a/AvanceBrico.xlsx
+++ b/AvanceBrico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\BDepBDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC53C4B-41CB-42F4-B081-6F79ACF472ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B798D3FE-FDF8-499B-B0E6-6FDD8E9074F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32070" yWindow="2160" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3880643-3CE2-4F0A-A429-8A0A59B669F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisateur non admin" sheetId="1" r:id="rId1"/>
@@ -4295,10 +4295,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CCEB15-3D11-4D0A-B678-DDAB2C4259D8}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="E5">
         <f>SUM(B:B)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="E7">
         <f>COUNTA(B:B)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
         <v>35</v>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="E13" s="7">
         <f>E5/E7</f>
-        <v>0.84848484848484851</v>
+        <v>0.91176470588235292</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
@@ -4710,11 +4710,11 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>512</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4726,11 +4726,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="4" t="s">
         <v>542</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4749,22 +4749,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>546</v>
       </c>
       <c r="B33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -4785,7 +4788,7 @@
   <sheetPr codeName="Feuil6"/>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>

</xml_diff>